<commit_message>
age and gender cohort calcs
</commit_message>
<xml_diff>
--- a/interx.xlsx
+++ b/interx.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="interx" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="59">
   <si>
     <t>GHT</t>
   </si>
@@ -127,6 +128,75 @@
   </si>
   <si>
     <t>Neither</t>
+  </si>
+  <si>
+    <t>OCT.Score</t>
+  </si>
+  <si>
+    <t>criterion</t>
+  </si>
+  <si>
+    <t>Repeat.Error.Rate</t>
+  </si>
+  <si>
+    <t>lower.CI</t>
+  </si>
+  <si>
+    <t>upper.CI</t>
+  </si>
+  <si>
+    <t>0\n45|36|22|22|15</t>
+  </si>
+  <si>
+    <t>1-3\n71|67|52|52|38</t>
+  </si>
+  <si>
+    <t>4-5\n39|39|36|36|31</t>
+  </si>
+  <si>
+    <t>6\n44|44|40|38|36</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>&gt;10%\n59|41|26|26|5</t>
+  </si>
+  <si>
+    <t>2-10%\n20|21|15|15|7</t>
+  </si>
+  <si>
+    <t>0.5-2%\n35|38|27|27|24</t>
+  </si>
+  <si>
+    <t>&lt;0.5%\n85|86|82|80|84</t>
+  </si>
+  <si>
+    <t>Hit.Rate</t>
+  </si>
+  <si>
+    <t>&gt;10%\nmed=-0.3dB\nN=584</t>
+  </si>
+  <si>
+    <t>2-10%\nmed=-2.1dB\nN=135</t>
+  </si>
+  <si>
+    <t>0.5-2%\nmed=-3.4dB\nN=169</t>
+  </si>
+  <si>
+    <t>&lt;0.5%\nmed=-7.3dB\nN=342</t>
+  </si>
+  <si>
+    <t>0\nmed=-0.8dB\nN=490</t>
+  </si>
+  <si>
+    <t>1-3\nmed=-1.9dB\nN=434</t>
+  </si>
+  <si>
+    <t>4-5\nmed=-5.3dB\nN=168</t>
+  </si>
+  <si>
+    <t>6\nmed=-7.4dB\nN=138</t>
   </si>
 </sst>
 </file>
@@ -652,7 +722,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -681,6 +751,7 @@
     <xf numFmtId="14" fontId="0" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1009,7 +1080,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK1231"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
@@ -9785,4 +9856,1607 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="P27" sqref="P27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="12" max="12" width="9.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="28">
+        <v>0.62</v>
+      </c>
+      <c r="E2" s="28">
+        <v>0.58503886999999999</v>
+      </c>
+      <c r="F2" s="28">
+        <v>0.66332740000000001</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="28">
+        <v>0.27</v>
+      </c>
+      <c r="L2" s="28">
+        <v>0.17436969999999999</v>
+      </c>
+      <c r="M2" s="28">
+        <v>0.39597763000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="28">
+        <v>0.87</v>
+      </c>
+      <c r="E3" s="28">
+        <v>0.80757714999999997</v>
+      </c>
+      <c r="F3" s="28">
+        <v>0.91987129999999995</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="28">
+        <v>0</v>
+      </c>
+      <c r="L3" s="28">
+        <v>1.1641729999999999E-17</v>
+      </c>
+      <c r="M3" s="28">
+        <v>0.16112515999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="28">
+        <v>0.95</v>
+      </c>
+      <c r="E4" s="28">
+        <v>0.90190013000000002</v>
+      </c>
+      <c r="F4" s="28">
+        <v>0.97173290000000001</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="28">
+        <v>0.03</v>
+      </c>
+      <c r="L4" s="28">
+        <v>5.0614919999999999E-3</v>
+      </c>
+      <c r="M4" s="28">
+        <v>0.14533087</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="28">
+        <v>1</v>
+      </c>
+      <c r="E5" s="28">
+        <v>0.98362576999999995</v>
+      </c>
+      <c r="F5" s="28">
+        <v>0.99948369999999997</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="28">
+        <v>0</v>
+      </c>
+      <c r="L5" s="28">
+        <v>0</v>
+      </c>
+      <c r="M5" s="28">
+        <v>4.3239479999999997E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="28">
+        <v>0.41</v>
+      </c>
+      <c r="E6" s="28">
+        <v>0.37008735999999998</v>
+      </c>
+      <c r="F6" s="28">
+        <v>0.44959189999999999</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" t="s">
+        <v>3</v>
+      </c>
+      <c r="K6" s="28">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="L6" s="28">
+        <v>0.1760919</v>
+      </c>
+      <c r="M6" s="28">
+        <v>0.44479468</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="28">
+        <v>0.99</v>
+      </c>
+      <c r="E7" s="28">
+        <v>0.95923592000000002</v>
+      </c>
+      <c r="F7" s="28">
+        <v>0.9986912</v>
+      </c>
+      <c r="H7">
+        <v>6</v>
+      </c>
+      <c r="I7" t="s">
+        <v>47</v>
+      </c>
+      <c r="J7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K7" s="28">
+        <v>0.05</v>
+      </c>
+      <c r="L7" s="28">
+        <v>8.4559879999999994E-3</v>
+      </c>
+      <c r="M7" s="28">
+        <v>0.2266936</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="28">
+        <v>1</v>
+      </c>
+      <c r="E8" s="28">
+        <v>0.97777466999999996</v>
+      </c>
+      <c r="F8" s="28">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>7</v>
+      </c>
+      <c r="I8" t="s">
+        <v>48</v>
+      </c>
+      <c r="J8" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" s="28">
+        <v>0.05</v>
+      </c>
+      <c r="L8" s="28">
+        <v>1.455421E-2</v>
+      </c>
+      <c r="M8" s="28">
+        <v>0.17285461999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="28">
+        <v>1</v>
+      </c>
+      <c r="E9" s="28">
+        <v>0.98889243000000004</v>
+      </c>
+      <c r="F9" s="28">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>8</v>
+      </c>
+      <c r="I9" t="s">
+        <v>49</v>
+      </c>
+      <c r="J9" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" s="28">
+        <v>0</v>
+      </c>
+      <c r="L9" s="28">
+        <v>3.3211E-18</v>
+      </c>
+      <c r="M9" s="28">
+        <v>4.2758200000000003E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="28">
+        <v>0.23</v>
+      </c>
+      <c r="E10" s="28">
+        <v>0.19395914</v>
+      </c>
+      <c r="F10" s="28">
+        <v>0.26167639999999998</v>
+      </c>
+      <c r="H10">
+        <v>9</v>
+      </c>
+      <c r="I10" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" t="s">
+        <v>0</v>
+      </c>
+      <c r="K10" s="28">
+        <v>0.35</v>
+      </c>
+      <c r="L10" s="28">
+        <v>0.1941223</v>
+      </c>
+      <c r="M10" s="28">
+        <v>0.53779429000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="28">
+        <v>0.53</v>
+      </c>
+      <c r="E11" s="28">
+        <v>0.44214895999999998</v>
+      </c>
+      <c r="F11" s="28">
+        <v>0.60826829999999998</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="I11" t="s">
+        <v>47</v>
+      </c>
+      <c r="J11" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11" s="28">
+        <v>0.27</v>
+      </c>
+      <c r="L11" s="28">
+        <v>0.1089745</v>
+      </c>
+      <c r="M11" s="28">
+        <v>0.51950434000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="28">
+        <v>0.69</v>
+      </c>
+      <c r="E12" s="28">
+        <v>0.61295613999999998</v>
+      </c>
+      <c r="F12" s="28">
+        <v>0.75153970000000003</v>
+      </c>
+      <c r="H12">
+        <v>11</v>
+      </c>
+      <c r="I12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J12" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12" s="28">
+        <v>0.26</v>
+      </c>
+      <c r="L12" s="28">
+        <v>0.13170370000000001</v>
+      </c>
+      <c r="M12" s="28">
+        <v>0.44678571</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="28">
+        <v>0.96</v>
+      </c>
+      <c r="E13" s="28">
+        <v>0.93968006000000004</v>
+      </c>
+      <c r="F13" s="28">
+        <v>0.97981640000000003</v>
+      </c>
+      <c r="H13">
+        <v>12</v>
+      </c>
+      <c r="I13" t="s">
+        <v>49</v>
+      </c>
+      <c r="J13" t="s">
+        <v>0</v>
+      </c>
+      <c r="K13" s="28">
+        <v>0.04</v>
+      </c>
+      <c r="L13" s="28">
+        <v>1.2519570000000001E-2</v>
+      </c>
+      <c r="M13" s="28">
+        <v>0.10212735000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="28">
+        <v>0.22</v>
+      </c>
+      <c r="E14" s="28">
+        <v>0.19073838000000001</v>
+      </c>
+      <c r="F14" s="28">
+        <v>0.25809260000000001</v>
+      </c>
+      <c r="H14">
+        <v>13</v>
+      </c>
+      <c r="I14" t="s">
+        <v>46</v>
+      </c>
+      <c r="J14" t="s">
+        <v>1</v>
+      </c>
+      <c r="K14" s="28">
+        <v>0.35</v>
+      </c>
+      <c r="L14" s="28">
+        <v>0.1941223</v>
+      </c>
+      <c r="M14" s="28">
+        <v>0.53779429000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="28">
+        <v>0.52</v>
+      </c>
+      <c r="E15" s="28">
+        <v>0.43489319999999998</v>
+      </c>
+      <c r="F15" s="28">
+        <v>0.60111910000000002</v>
+      </c>
+      <c r="H15">
+        <v>14</v>
+      </c>
+      <c r="I15" t="s">
+        <v>47</v>
+      </c>
+      <c r="J15" t="s">
+        <v>1</v>
+      </c>
+      <c r="K15" s="28">
+        <v>0.27</v>
+      </c>
+      <c r="L15" s="28">
+        <v>0.1089745</v>
+      </c>
+      <c r="M15" s="28">
+        <v>0.51950434000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="28">
+        <v>0.69</v>
+      </c>
+      <c r="E16" s="28">
+        <v>0.61295613999999998</v>
+      </c>
+      <c r="F16" s="28">
+        <v>0.75153970000000003</v>
+      </c>
+      <c r="H16">
+        <v>15</v>
+      </c>
+      <c r="I16" t="s">
+        <v>48</v>
+      </c>
+      <c r="J16" t="s">
+        <v>1</v>
+      </c>
+      <c r="K16" s="28">
+        <v>0.26</v>
+      </c>
+      <c r="L16" s="28">
+        <v>0.13170370000000001</v>
+      </c>
+      <c r="M16" s="28">
+        <v>0.44678571</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="28">
+        <v>0.9</v>
+      </c>
+      <c r="E17" s="28">
+        <v>0.86099603000000002</v>
+      </c>
+      <c r="F17" s="28">
+        <v>0.92549150000000002</v>
+      </c>
+      <c r="H17">
+        <v>16</v>
+      </c>
+      <c r="I17" t="s">
+        <v>49</v>
+      </c>
+      <c r="J17" t="s">
+        <v>1</v>
+      </c>
+      <c r="K17" s="28">
+        <v>0.04</v>
+      </c>
+      <c r="L17" s="28">
+        <v>1.283457E-2</v>
+      </c>
+      <c r="M17" s="28">
+        <v>0.10454720000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="28">
+        <v>0.03</v>
+      </c>
+      <c r="E18" s="28">
+        <v>2.2277020000000002E-2</v>
+      </c>
+      <c r="F18" s="28">
+        <v>5.23034E-2</v>
+      </c>
+      <c r="H18">
+        <v>17</v>
+      </c>
+      <c r="I18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J18" t="s">
+        <v>2</v>
+      </c>
+      <c r="K18" s="28">
+        <v>0.4</v>
+      </c>
+      <c r="L18" s="28">
+        <v>0.1176208</v>
+      </c>
+      <c r="M18" s="28">
+        <v>0.76927572</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="28">
+        <v>0.24</v>
+      </c>
+      <c r="E19" s="28">
+        <v>0.17968181999999999</v>
+      </c>
+      <c r="F19" s="28">
+        <v>0.32334849999999998</v>
+      </c>
+      <c r="H19">
+        <v>18</v>
+      </c>
+      <c r="I19" t="s">
+        <v>47</v>
+      </c>
+      <c r="J19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K19" s="28">
+        <v>0.43</v>
+      </c>
+      <c r="L19" s="28">
+        <v>0.1582199</v>
+      </c>
+      <c r="M19" s="28">
+        <v>0.74954164000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="28">
+        <v>0.5</v>
+      </c>
+      <c r="E20" s="28">
+        <v>0.42835329</v>
+      </c>
+      <c r="F20" s="28">
+        <v>0.57743239999999996</v>
+      </c>
+      <c r="H20">
+        <v>19</v>
+      </c>
+      <c r="I20" t="s">
+        <v>48</v>
+      </c>
+      <c r="J20" t="s">
+        <v>2</v>
+      </c>
+      <c r="K20" s="28">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="L20" s="28">
+        <v>0.14914649999999999</v>
+      </c>
+      <c r="M20" s="28">
+        <v>0.49167694000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="28">
+        <v>0.97</v>
+      </c>
+      <c r="E21" s="28">
+        <v>0.94333237000000003</v>
+      </c>
+      <c r="F21" s="28">
+        <v>0.98194709999999996</v>
+      </c>
+      <c r="H21">
+        <v>20</v>
+      </c>
+      <c r="I21" t="s">
+        <v>49</v>
+      </c>
+      <c r="J21" t="s">
+        <v>2</v>
+      </c>
+      <c r="K21" s="28">
+        <v>0.08</v>
+      </c>
+      <c r="L21" s="28">
+        <v>4.0952549999999997E-2</v>
+      </c>
+      <c r="M21" s="28">
+        <v>0.16215721999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" t="s">
+        <v>40</v>
+      </c>
+      <c r="I23" t="s">
+        <v>36</v>
+      </c>
+      <c r="J23" t="s">
+        <v>37</v>
+      </c>
+      <c r="K23" t="s">
+        <v>38</v>
+      </c>
+      <c r="L23" t="s">
+        <v>39</v>
+      </c>
+      <c r="M23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="28">
+        <v>0.64</v>
+      </c>
+      <c r="E24" s="28">
+        <v>0.59947099999999998</v>
+      </c>
+      <c r="F24" s="28">
+        <v>0.68402079999999998</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24" t="s">
+        <v>41</v>
+      </c>
+      <c r="J24" t="s">
+        <v>7</v>
+      </c>
+      <c r="K24" s="28">
+        <v>0.36</v>
+      </c>
+      <c r="L24" s="28">
+        <v>0.2321908</v>
+      </c>
+      <c r="M24" s="28">
+        <v>0.50164185999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="28">
+        <v>0.85</v>
+      </c>
+      <c r="E25" s="28">
+        <v>0.81858330000000001</v>
+      </c>
+      <c r="F25" s="28">
+        <v>0.88486770000000003</v>
+      </c>
+      <c r="H25">
+        <v>2</v>
+      </c>
+      <c r="I25" t="s">
+        <v>42</v>
+      </c>
+      <c r="J25" t="s">
+        <v>7</v>
+      </c>
+      <c r="K25" s="28">
+        <v>0.01</v>
+      </c>
+      <c r="L25" s="28">
+        <v>2.4906030000000001E-3</v>
+      </c>
+      <c r="M25" s="28">
+        <v>7.5560509999999997E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="28">
+        <v>0.95</v>
+      </c>
+      <c r="E26" s="28">
+        <v>0.90886020000000001</v>
+      </c>
+      <c r="F26" s="28">
+        <v>0.97567599999999999</v>
+      </c>
+      <c r="H26">
+        <v>3</v>
+      </c>
+      <c r="I26" t="s">
+        <v>43</v>
+      </c>
+      <c r="J26" t="s">
+        <v>7</v>
+      </c>
+      <c r="K26" s="28">
+        <v>0</v>
+      </c>
+      <c r="L26" s="28">
+        <v>0</v>
+      </c>
+      <c r="M26" s="28">
+        <v>8.9666850000000006E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>4</v>
+      </c>
+      <c r="B27" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="28">
+        <v>1</v>
+      </c>
+      <c r="E27" s="28">
+        <v>0.97291720000000004</v>
+      </c>
+      <c r="F27" s="28">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>4</v>
+      </c>
+      <c r="I27" t="s">
+        <v>44</v>
+      </c>
+      <c r="J27" t="s">
+        <v>7</v>
+      </c>
+      <c r="K27" s="28">
+        <v>0</v>
+      </c>
+      <c r="L27" s="28">
+        <v>0</v>
+      </c>
+      <c r="M27" s="28">
+        <v>8.0295599999999995E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="28">
+        <v>0.52</v>
+      </c>
+      <c r="E28" s="28">
+        <v>0.47821989999999998</v>
+      </c>
+      <c r="F28" s="28">
+        <v>0.56632879999999997</v>
+      </c>
+      <c r="H28">
+        <v>5</v>
+      </c>
+      <c r="I28" t="s">
+        <v>41</v>
+      </c>
+      <c r="J28" t="s">
+        <v>3</v>
+      </c>
+      <c r="K28" s="28">
+        <v>0.22</v>
+      </c>
+      <c r="L28" s="28">
+        <v>0.1171633</v>
+      </c>
+      <c r="M28" s="28">
+        <v>0.38084702999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>6</v>
+      </c>
+      <c r="B29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="28">
+        <v>0.77</v>
+      </c>
+      <c r="E29" s="28">
+        <v>0.72770590000000002</v>
+      </c>
+      <c r="F29" s="28">
+        <v>0.80673419999999996</v>
+      </c>
+      <c r="H29">
+        <v>6</v>
+      </c>
+      <c r="I29" t="s">
+        <v>42</v>
+      </c>
+      <c r="J29" t="s">
+        <v>3</v>
+      </c>
+      <c r="K29" s="28">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L29" s="28">
+        <v>3.229605E-2</v>
+      </c>
+      <c r="M29" s="28">
+        <v>0.16309037000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>7</v>
+      </c>
+      <c r="B30" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="28">
+        <v>0.93</v>
+      </c>
+      <c r="E30" s="28">
+        <v>0.8865712</v>
+      </c>
+      <c r="F30" s="28">
+        <v>0.96304909999999999</v>
+      </c>
+      <c r="H30">
+        <v>7</v>
+      </c>
+      <c r="I30" t="s">
+        <v>43</v>
+      </c>
+      <c r="J30" t="s">
+        <v>3</v>
+      </c>
+      <c r="K30" s="28">
+        <v>0.03</v>
+      </c>
+      <c r="L30" s="28">
+        <v>4.5407030000000001E-3</v>
+      </c>
+      <c r="M30" s="28">
+        <v>0.13180990000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>8</v>
+      </c>
+      <c r="B31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31" s="28">
+        <v>0.99</v>
+      </c>
+      <c r="E31" s="28">
+        <v>0.96009730000000004</v>
+      </c>
+      <c r="F31" s="28">
+        <v>0.99871969999999999</v>
+      </c>
+      <c r="H31">
+        <v>8</v>
+      </c>
+      <c r="I31" t="s">
+        <v>44</v>
+      </c>
+      <c r="J31" t="s">
+        <v>3</v>
+      </c>
+      <c r="K31" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="L31" s="28">
+        <v>4.0232519999999997E-3</v>
+      </c>
+      <c r="M31" s="28">
+        <v>0.1180771</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>9</v>
+      </c>
+      <c r="B32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32" s="28">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E32" s="28">
+        <v>0.2533282</v>
+      </c>
+      <c r="F32" s="28">
+        <v>0.33358369999999998</v>
+      </c>
+      <c r="H32">
+        <v>9</v>
+      </c>
+      <c r="I32" t="s">
+        <v>41</v>
+      </c>
+      <c r="J32" t="s">
+        <v>0</v>
+      </c>
+      <c r="K32" s="28">
+        <v>0.18</v>
+      </c>
+      <c r="L32" s="28">
+        <v>7.3068850000000005E-2</v>
+      </c>
+      <c r="M32" s="28">
+        <v>0.38516607000000003</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>10</v>
+      </c>
+      <c r="B33" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33" s="28">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E33" s="28">
+        <v>0.4990424</v>
+      </c>
+      <c r="F33" s="28">
+        <v>0.59231489999999998</v>
+      </c>
+      <c r="H33">
+        <v>10</v>
+      </c>
+      <c r="I33" t="s">
+        <v>42</v>
+      </c>
+      <c r="J33" t="s">
+        <v>0</v>
+      </c>
+      <c r="K33" s="28">
+        <v>0.31</v>
+      </c>
+      <c r="L33" s="28">
+        <v>0.1991473</v>
+      </c>
+      <c r="M33" s="28">
+        <v>0.44269588999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>11</v>
+      </c>
+      <c r="B34" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34" s="28">
+        <v>0.83</v>
+      </c>
+      <c r="E34" s="28">
+        <v>0.76966489999999999</v>
+      </c>
+      <c r="F34" s="28">
+        <v>0.88209870000000001</v>
+      </c>
+      <c r="H34">
+        <v>11</v>
+      </c>
+      <c r="I34" t="s">
+        <v>43</v>
+      </c>
+      <c r="J34" t="s">
+        <v>0</v>
+      </c>
+      <c r="K34" s="28">
+        <v>0.08</v>
+      </c>
+      <c r="L34" s="28">
+        <v>2.8748610000000001E-2</v>
+      </c>
+      <c r="M34" s="28">
+        <v>0.21826691000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>12</v>
+      </c>
+      <c r="B35" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35" s="28">
+        <v>0.93</v>
+      </c>
+      <c r="E35" s="28">
+        <v>0.88070230000000005</v>
+      </c>
+      <c r="F35" s="28">
+        <v>0.96531270000000002</v>
+      </c>
+      <c r="H35">
+        <v>12</v>
+      </c>
+      <c r="I35" t="s">
+        <v>44</v>
+      </c>
+      <c r="J35" t="s">
+        <v>0</v>
+      </c>
+      <c r="K35" s="28">
+        <v>0</v>
+      </c>
+      <c r="L35" s="28">
+        <v>6.3308969999999999E-18</v>
+      </c>
+      <c r="M35" s="28">
+        <v>8.7621599999999994E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>13</v>
+      </c>
+      <c r="B36" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" s="28">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E36" s="28">
+        <v>0.24944369999999999</v>
+      </c>
+      <c r="F36" s="28">
+        <v>0.32936850000000001</v>
+      </c>
+      <c r="H36">
+        <v>13</v>
+      </c>
+      <c r="I36" t="s">
+        <v>41</v>
+      </c>
+      <c r="J36" t="s">
+        <v>1</v>
+      </c>
+      <c r="K36" s="28">
+        <v>0.18</v>
+      </c>
+      <c r="L36" s="28">
+        <v>7.3068850000000005E-2</v>
+      </c>
+      <c r="M36" s="28">
+        <v>0.38516607000000003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>14</v>
+      </c>
+      <c r="B37" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" s="28">
+        <v>0.54</v>
+      </c>
+      <c r="E37" s="28">
+        <v>0.49443690000000001</v>
+      </c>
+      <c r="F37" s="28">
+        <v>0.58778459999999999</v>
+      </c>
+      <c r="H37">
+        <v>14</v>
+      </c>
+      <c r="I37" t="s">
+        <v>42</v>
+      </c>
+      <c r="J37" t="s">
+        <v>1</v>
+      </c>
+      <c r="K37" s="28">
+        <v>0.31</v>
+      </c>
+      <c r="L37" s="28">
+        <v>0.1991473</v>
+      </c>
+      <c r="M37" s="28">
+        <v>0.44269588999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>15</v>
+      </c>
+      <c r="B38" t="s">
+        <v>57</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" s="28">
+        <v>0.79</v>
+      </c>
+      <c r="E38" s="28">
+        <v>0.71764589999999995</v>
+      </c>
+      <c r="F38" s="28">
+        <v>0.8410086</v>
+      </c>
+      <c r="H38">
+        <v>15</v>
+      </c>
+      <c r="I38" t="s">
+        <v>43</v>
+      </c>
+      <c r="J38" t="s">
+        <v>1</v>
+      </c>
+      <c r="K38" s="28">
+        <v>0.08</v>
+      </c>
+      <c r="L38" s="28">
+        <v>2.8748610000000001E-2</v>
+      </c>
+      <c r="M38" s="28">
+        <v>0.21826691000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>16</v>
+      </c>
+      <c r="B39" t="s">
+        <v>58</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" s="28">
+        <v>0.83</v>
+      </c>
+      <c r="E39" s="28">
+        <v>0.76231389999999999</v>
+      </c>
+      <c r="F39" s="28">
+        <v>0.88629760000000002</v>
+      </c>
+      <c r="H39">
+        <v>16</v>
+      </c>
+      <c r="I39" t="s">
+        <v>44</v>
+      </c>
+      <c r="J39" t="s">
+        <v>1</v>
+      </c>
+      <c r="K39" s="28">
+        <v>0</v>
+      </c>
+      <c r="L39" s="28">
+        <v>0</v>
+      </c>
+      <c r="M39" s="28">
+        <v>9.1809870000000002E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>17</v>
+      </c>
+      <c r="B40" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" s="28">
+        <v>0.16</v>
+      </c>
+      <c r="E40" s="28">
+        <v>0.1294594</v>
+      </c>
+      <c r="F40" s="28">
+        <v>0.1942102</v>
+      </c>
+      <c r="H40">
+        <v>17</v>
+      </c>
+      <c r="I40" t="s">
+        <v>41</v>
+      </c>
+      <c r="J40" t="s">
+        <v>2</v>
+      </c>
+      <c r="K40" s="28">
+        <v>0.33</v>
+      </c>
+      <c r="L40" s="28">
+        <v>0.15176319999999999</v>
+      </c>
+      <c r="M40" s="28">
+        <v>0.58286452</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>18</v>
+      </c>
+      <c r="B41" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" s="28">
+        <v>0.37</v>
+      </c>
+      <c r="E41" s="28">
+        <v>0.32238679999999997</v>
+      </c>
+      <c r="F41" s="28">
+        <v>0.41267710000000002</v>
+      </c>
+      <c r="H41">
+        <v>18</v>
+      </c>
+      <c r="I41" t="s">
+        <v>42</v>
+      </c>
+      <c r="J41" t="s">
+        <v>2</v>
+      </c>
+      <c r="K41" s="28">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="L41" s="28">
+        <v>0.17003280000000001</v>
+      </c>
+      <c r="M41" s="28">
+        <v>0.44757138000000002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>19</v>
+      </c>
+      <c r="B42" t="s">
+        <v>57</v>
+      </c>
+      <c r="C42" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" s="28">
+        <v>0.68</v>
+      </c>
+      <c r="E42" s="28">
+        <v>0.61079620000000001</v>
+      </c>
+      <c r="F42" s="28">
+        <v>0.75000149999999999</v>
+      </c>
+      <c r="H42">
+        <v>19</v>
+      </c>
+      <c r="I42" t="s">
+        <v>43</v>
+      </c>
+      <c r="J42" t="s">
+        <v>2</v>
+      </c>
+      <c r="K42" s="28">
+        <v>0</v>
+      </c>
+      <c r="L42" s="28">
+        <v>0</v>
+      </c>
+      <c r="M42" s="28">
+        <v>0.1102554</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>20</v>
+      </c>
+      <c r="B43" t="s">
+        <v>58</v>
+      </c>
+      <c r="C43" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" s="28">
+        <v>0.85</v>
+      </c>
+      <c r="E43" s="28">
+        <v>0.77854889999999999</v>
+      </c>
+      <c r="F43" s="28">
+        <v>0.89826309999999998</v>
+      </c>
+      <c r="H43">
+        <v>20</v>
+      </c>
+      <c r="I43" t="s">
+        <v>44</v>
+      </c>
+      <c r="J43" t="s">
+        <v>2</v>
+      </c>
+      <c r="K43" s="28">
+        <v>0.08</v>
+      </c>
+      <c r="L43" s="28">
+        <v>2.8748610000000001E-2</v>
+      </c>
+      <c r="M43" s="28">
+        <v>0.21826691000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>